<commit_message>
refs #12 Business rule file modified
</commit_message>
<xml_diff>
--- a/tests/Test_Project/【ビジネスルール】_ビジネスルール一覧.xlsx
+++ b/tests/Test_Project/【ビジネスルール】_ビジネスルール一覧.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,14 +15,59 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -34,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,18 +87,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,37 +414,662 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2">
+        <v>14</v>
+      </c>
+      <c r="F15" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2">
+        <v>15</v>
+      </c>
+      <c r="F16" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2">
+        <v>17</v>
+      </c>
+      <c r="E18" s="2">
+        <v>17</v>
+      </c>
+      <c r="F18" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>18</v>
+      </c>
+      <c r="F19" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2">
+        <v>19</v>
+      </c>
+      <c r="D20" s="2">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2">
+        <v>19</v>
+      </c>
+      <c r="F20" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2">
+        <v>20</v>
+      </c>
+      <c r="D21" s="2">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
+        <v>20</v>
+      </c>
+      <c r="F21" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2">
+        <v>21</v>
+      </c>
+      <c r="E22" s="2">
+        <v>21</v>
+      </c>
+      <c r="F22" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2">
+        <v>22</v>
+      </c>
+      <c r="E23" s="2">
+        <v>22</v>
+      </c>
+      <c r="F23" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2">
+        <v>23</v>
+      </c>
+      <c r="D24" s="2">
+        <v>23</v>
+      </c>
+      <c r="E24" s="2">
+        <v>23</v>
+      </c>
+      <c r="F24" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2">
+        <v>24</v>
+      </c>
+      <c r="D25" s="2">
+        <v>24</v>
+      </c>
+      <c r="E25" s="2">
+        <v>24</v>
+      </c>
+      <c r="F25" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>25</v>
+      </c>
+      <c r="C26" s="2">
+        <v>25</v>
+      </c>
+      <c r="D26" s="2">
+        <v>25</v>
+      </c>
+      <c r="E26" s="2">
+        <v>25</v>
+      </c>
+      <c r="F26" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>26</v>
+      </c>
+      <c r="C27" s="2">
+        <v>26</v>
+      </c>
+      <c r="D27" s="2">
+        <v>26</v>
+      </c>
+      <c r="E27" s="2">
+        <v>26</v>
+      </c>
+      <c r="F27" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2">
+        <v>27</v>
+      </c>
+      <c r="D28" s="2">
+        <v>27</v>
+      </c>
+      <c r="E28" s="2">
+        <v>27</v>
+      </c>
+      <c r="F28" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>28</v>
+      </c>
+      <c r="C29" s="2">
+        <v>28</v>
+      </c>
+      <c r="D29" s="2">
+        <v>28</v>
+      </c>
+      <c r="E29" s="2">
+        <v>28</v>
+      </c>
+      <c r="F29" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>29</v>
+      </c>
+      <c r="C30" s="2">
+        <v>29</v>
+      </c>
+      <c r="D30" s="2">
+        <v>29</v>
+      </c>
+      <c r="E30" s="2">
+        <v>29</v>
+      </c>
+      <c r="F30" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>30</v>
+      </c>
+      <c r="C31" s="2">
+        <v>30</v>
+      </c>
+      <c r="D31" s="2">
+        <v>30</v>
+      </c>
+      <c r="E31" s="2">
+        <v>30</v>
+      </c>
+      <c r="F31" s="2">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>